<commit_message>
Final excel to email project
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonidas Petrou\Documents\UiPath\project2_rpacrm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\UiPath\RepProject1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86223B16-5327-465F-ADC2-EA58D614E75E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4836A408-A0F2-4ACC-9BBE-3075103C458F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7476" windowHeight="5568" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="829">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2018" uniqueCount="933">
   <si>
     <t>first name</t>
   </si>
@@ -2507,6 +2508,318 @@
   </si>
   <si>
     <t>bphilipps2r@indiegogo.com</t>
+  </si>
+  <si>
+    <t>full name</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>GWENDOLIN FERROLLI</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>THAYNE DE LASCI</t>
+  </si>
+  <si>
+    <t>Not Success</t>
+  </si>
+  <si>
+    <t>CRISTINE ROMEO</t>
+  </si>
+  <si>
+    <t>CHERIE BRELLIN</t>
+  </si>
+  <si>
+    <t>PEGGY HELLIAR</t>
+  </si>
+  <si>
+    <t>ADDISON GENTERY</t>
+  </si>
+  <si>
+    <t>ROBINET DORRIAN</t>
+  </si>
+  <si>
+    <t>SHERWIN RUSHBROOKE</t>
+  </si>
+  <si>
+    <t>MARTHE GOLIGHTLY</t>
+  </si>
+  <si>
+    <t>AUSTIN LEYBAND</t>
+  </si>
+  <si>
+    <t>KINSLEY WHIMPER</t>
+  </si>
+  <si>
+    <t>ONOFREDO TILZEY</t>
+  </si>
+  <si>
+    <t>SHELBY MCGILLEGHOLE</t>
+  </si>
+  <si>
+    <t>GABIE PAVLOV</t>
+  </si>
+  <si>
+    <t>LETTY MCKEURTON</t>
+  </si>
+  <si>
+    <t>HAZLETT THYNG</t>
+  </si>
+  <si>
+    <t>SONNY DANKERSLEY</t>
+  </si>
+  <si>
+    <t>NERITA VAN OORD</t>
+  </si>
+  <si>
+    <t>MELITA ANSLEY</t>
+  </si>
+  <si>
+    <t>DOTTI MCELWEE</t>
+  </si>
+  <si>
+    <t>CALEB BROOKSON</t>
+  </si>
+  <si>
+    <t>CARMINA CASTIGLIONI</t>
+  </si>
+  <si>
+    <t>LAETITIA SABBINS</t>
+  </si>
+  <si>
+    <t>CHUCHO DAMEISELE</t>
+  </si>
+  <si>
+    <t>THEOBALD ROLLINGS</t>
+  </si>
+  <si>
+    <t>ROBBIE MCCRITICHIE</t>
+  </si>
+  <si>
+    <t>WESTBROOK HILARY</t>
+  </si>
+  <si>
+    <t>JAQUITH MCVANAMY</t>
+  </si>
+  <si>
+    <t>KATUSHA SIEMENS</t>
+  </si>
+  <si>
+    <t>MARCELLE MOORWOOD</t>
+  </si>
+  <si>
+    <t>DONNY CHARMAN</t>
+  </si>
+  <si>
+    <t>HEATHER WARHAM</t>
+  </si>
+  <si>
+    <t>CHRISTOPHER GIURIO</t>
+  </si>
+  <si>
+    <t>BOBBEE PIDCOCK</t>
+  </si>
+  <si>
+    <t>SEAMUS SOKELL</t>
+  </si>
+  <si>
+    <t>TODD YURIN</t>
+  </si>
+  <si>
+    <t>CHRISSE TYLOR</t>
+  </si>
+  <si>
+    <t>MARGERY INNETT</t>
+  </si>
+  <si>
+    <t>DONNAJEAN SIBBERING</t>
+  </si>
+  <si>
+    <t>CONNY MYTTON</t>
+  </si>
+  <si>
+    <t>KILEY FINLEY</t>
+  </si>
+  <si>
+    <t>GOLDIA THORPE</t>
+  </si>
+  <si>
+    <t>CHARLENE AHREN</t>
+  </si>
+  <si>
+    <t>HALE FORRI</t>
+  </si>
+  <si>
+    <t>REBA DI ROCCA</t>
+  </si>
+  <si>
+    <t>VINCENTY GOODSAL</t>
+  </si>
+  <si>
+    <t>JULIANNE MACAK</t>
+  </si>
+  <si>
+    <t>RORA PARTLETT</t>
+  </si>
+  <si>
+    <t>ZEBULON BARNWILL</t>
+  </si>
+  <si>
+    <t>TAN HEANEY`</t>
+  </si>
+  <si>
+    <t>BERNI BARNABY</t>
+  </si>
+  <si>
+    <t>ABBY DUCKET</t>
+  </si>
+  <si>
+    <t>DERREK SOLDAN</t>
+  </si>
+  <si>
+    <t>COLET BULLAR</t>
+  </si>
+  <si>
+    <t>KINSLEY TATTERSILL</t>
+  </si>
+  <si>
+    <t>KATHERINE GILLOW</t>
+  </si>
+  <si>
+    <t>NANETTE MCGINTY</t>
+  </si>
+  <si>
+    <t>MUFFIN THYING</t>
+  </si>
+  <si>
+    <t>DEERDRE RADOUX</t>
+  </si>
+  <si>
+    <t>MIKEL VELLA</t>
+  </si>
+  <si>
+    <t>ALLISTIR DOCHON</t>
+  </si>
+  <si>
+    <t>LOUELLA FILIPPAZZO</t>
+  </si>
+  <si>
+    <t>CARESSA VONDRACEK</t>
+  </si>
+  <si>
+    <t>ARIANA BARZEN</t>
+  </si>
+  <si>
+    <t>LENCI ALES</t>
+  </si>
+  <si>
+    <t>JERAMEY FEARNEY</t>
+  </si>
+  <si>
+    <t>MELISANDE CONAGHY</t>
+  </si>
+  <si>
+    <t>ARRON GERRETSEN</t>
+  </si>
+  <si>
+    <t>BRITTAN FARREIL</t>
+  </si>
+  <si>
+    <t>ALAIR LONGSTAFF</t>
+  </si>
+  <si>
+    <t>KANIA CLAC</t>
+  </si>
+  <si>
+    <t>DERK SERRIS</t>
+  </si>
+  <si>
+    <t>GARV TUNMORE</t>
+  </si>
+  <si>
+    <t>PERCEVAL WORGAN</t>
+  </si>
+  <si>
+    <t>IRVIN LIVER</t>
+  </si>
+  <si>
+    <t>CORDELL LINFIELD</t>
+  </si>
+  <si>
+    <t>PATTON BARTOSIK</t>
+  </si>
+  <si>
+    <t>AUDRE JAMIESON</t>
+  </si>
+  <si>
+    <t>FREDRIC SLEIGHTHOLM</t>
+  </si>
+  <si>
+    <t>ROUVIN IVERMEE</t>
+  </si>
+  <si>
+    <t>LURETTE GRAVELL</t>
+  </si>
+  <si>
+    <t>RAOUL BATTIN</t>
+  </si>
+  <si>
+    <t>ROWLAND REXWORTHY</t>
+  </si>
+  <si>
+    <t>DORIS GARVAGH</t>
+  </si>
+  <si>
+    <t>DENNY BRITTONER</t>
+  </si>
+  <si>
+    <t>SELLE SEABROOK</t>
+  </si>
+  <si>
+    <t>BILLIE HABERSHAW</t>
+  </si>
+  <si>
+    <t>FEODORA COMI</t>
+  </si>
+  <si>
+    <t>JOELLE BUSEN</t>
+  </si>
+  <si>
+    <t>ROYAL JOIST</t>
+  </si>
+  <si>
+    <t>YOLANE COSSEM</t>
+  </si>
+  <si>
+    <t>BETSEY HAIR</t>
+  </si>
+  <si>
+    <t>ZACHARIA CATTO</t>
+  </si>
+  <si>
+    <t>NOELL THORNE</t>
+  </si>
+  <si>
+    <t>CHESTON ROBARTS</t>
+  </si>
+  <si>
+    <t>SHOLOM WHITTLESEE</t>
+  </si>
+  <si>
+    <t>SANSON DANAHER</t>
+  </si>
+  <si>
+    <t>GARDNER COWLAM</t>
+  </si>
+  <si>
+    <t>VERENA TARREN</t>
+  </si>
+  <si>
+    <t>BRAD PHILIPPS</t>
   </si>
 </sst>
 </file>
@@ -3346,27 +3659,3272 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F700AF1D-CE63-4620-84CF-277FA66D4361}">
+  <dimension ref="A1:J101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>829</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>831</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>833</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>835</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>836</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>837</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I6" t="s">
+        <v>55</v>
+      </c>
+      <c r="J6" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>838</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I7" t="s">
+        <v>64</v>
+      </c>
+      <c r="J7" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>839</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G8" t="s">
+        <v>71</v>
+      </c>
+      <c r="H8" t="s">
+        <v>72</v>
+      </c>
+      <c r="I8" t="s">
+        <v>73</v>
+      </c>
+      <c r="J8" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>840</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9" t="s">
+        <v>80</v>
+      </c>
+      <c r="H9" t="s">
+        <v>81</v>
+      </c>
+      <c r="I9" t="s">
+        <v>82</v>
+      </c>
+      <c r="J9" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>841</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10" t="s">
+        <v>87</v>
+      </c>
+      <c r="F10" t="s">
+        <v>88</v>
+      </c>
+      <c r="G10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H10" t="s">
+        <v>90</v>
+      </c>
+      <c r="I10" t="s">
+        <v>91</v>
+      </c>
+      <c r="J10" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>842</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" t="s">
+        <v>96</v>
+      </c>
+      <c r="F11" t="s">
+        <v>97</v>
+      </c>
+      <c r="G11" t="s">
+        <v>98</v>
+      </c>
+      <c r="H11" t="s">
+        <v>99</v>
+      </c>
+      <c r="I11" t="s">
+        <v>100</v>
+      </c>
+      <c r="J11" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>843</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" t="s">
+        <v>104</v>
+      </c>
+      <c r="E12" t="s">
+        <v>105</v>
+      </c>
+      <c r="F12" t="s">
+        <v>106</v>
+      </c>
+      <c r="G12" t="s">
+        <v>107</v>
+      </c>
+      <c r="H12" t="s">
+        <v>108</v>
+      </c>
+      <c r="I12" t="s">
+        <v>109</v>
+      </c>
+      <c r="J12" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>844</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D13" t="s">
+        <v>113</v>
+      </c>
+      <c r="E13" t="s">
+        <v>114</v>
+      </c>
+      <c r="F13" t="s">
+        <v>115</v>
+      </c>
+      <c r="G13" t="s">
+        <v>116</v>
+      </c>
+      <c r="H13" t="s">
+        <v>117</v>
+      </c>
+      <c r="I13" t="s">
+        <v>118</v>
+      </c>
+      <c r="J13" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>845</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>121</v>
+      </c>
+      <c r="D14" t="s">
+        <v>122</v>
+      </c>
+      <c r="E14" t="s">
+        <v>123</v>
+      </c>
+      <c r="F14" t="s">
+        <v>124</v>
+      </c>
+      <c r="G14" t="s">
+        <v>125</v>
+      </c>
+      <c r="H14" t="s">
+        <v>126</v>
+      </c>
+      <c r="I14" t="s">
+        <v>127</v>
+      </c>
+      <c r="J14" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>846</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>130</v>
+      </c>
+      <c r="D15" t="s">
+        <v>131</v>
+      </c>
+      <c r="E15" t="s">
+        <v>132</v>
+      </c>
+      <c r="F15" t="s">
+        <v>133</v>
+      </c>
+      <c r="G15" t="s">
+        <v>134</v>
+      </c>
+      <c r="H15" t="s">
+        <v>135</v>
+      </c>
+      <c r="I15" t="s">
+        <v>136</v>
+      </c>
+      <c r="J15" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>847</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>139</v>
+      </c>
+      <c r="D16" t="s">
+        <v>140</v>
+      </c>
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" t="s">
+        <v>141</v>
+      </c>
+      <c r="G16" t="s">
+        <v>142</v>
+      </c>
+      <c r="H16" t="s">
+        <v>143</v>
+      </c>
+      <c r="I16" t="s">
+        <v>144</v>
+      </c>
+      <c r="J16" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>848</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" t="s">
+        <v>147</v>
+      </c>
+      <c r="D17" t="s">
+        <v>148</v>
+      </c>
+      <c r="E17" t="s">
+        <v>149</v>
+      </c>
+      <c r="F17" t="s">
+        <v>150</v>
+      </c>
+      <c r="G17" t="s">
+        <v>151</v>
+      </c>
+      <c r="H17" t="s">
+        <v>152</v>
+      </c>
+      <c r="I17" t="s">
+        <v>153</v>
+      </c>
+      <c r="J17" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>849</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" t="s">
+        <v>156</v>
+      </c>
+      <c r="D18" t="s">
+        <v>157</v>
+      </c>
+      <c r="E18" t="s">
+        <v>158</v>
+      </c>
+      <c r="F18" t="s">
+        <v>159</v>
+      </c>
+      <c r="G18" t="s">
+        <v>160</v>
+      </c>
+      <c r="H18" t="s">
+        <v>161</v>
+      </c>
+      <c r="I18" t="s">
+        <v>162</v>
+      </c>
+      <c r="J18" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>850</v>
+      </c>
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" t="s">
+        <v>165</v>
+      </c>
+      <c r="D19" t="s">
+        <v>166</v>
+      </c>
+      <c r="E19" t="s">
+        <v>96</v>
+      </c>
+      <c r="F19" t="s">
+        <v>167</v>
+      </c>
+      <c r="G19" t="s">
+        <v>168</v>
+      </c>
+      <c r="H19" t="s">
+        <v>169</v>
+      </c>
+      <c r="I19" t="s">
+        <v>170</v>
+      </c>
+      <c r="J19" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>851</v>
+      </c>
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" t="s">
+        <v>173</v>
+      </c>
+      <c r="D20" t="s">
+        <v>174</v>
+      </c>
+      <c r="E20" t="s">
+        <v>175</v>
+      </c>
+      <c r="F20" t="s">
+        <v>176</v>
+      </c>
+      <c r="G20" t="s">
+        <v>177</v>
+      </c>
+      <c r="H20" t="s">
+        <v>178</v>
+      </c>
+      <c r="I20" t="s">
+        <v>179</v>
+      </c>
+      <c r="J20" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>852</v>
+      </c>
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" t="s">
+        <v>182</v>
+      </c>
+      <c r="D21" t="s">
+        <v>183</v>
+      </c>
+      <c r="E21" t="s">
+        <v>123</v>
+      </c>
+      <c r="F21" t="s">
+        <v>184</v>
+      </c>
+      <c r="G21" t="s">
+        <v>185</v>
+      </c>
+      <c r="H21" t="s">
+        <v>186</v>
+      </c>
+      <c r="I21" t="s">
+        <v>187</v>
+      </c>
+      <c r="J21" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>853</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" t="s">
+        <v>190</v>
+      </c>
+      <c r="D22" t="s">
+        <v>191</v>
+      </c>
+      <c r="E22" t="s">
+        <v>192</v>
+      </c>
+      <c r="F22" t="s">
+        <v>193</v>
+      </c>
+      <c r="G22" t="s">
+        <v>194</v>
+      </c>
+      <c r="H22" t="s">
+        <v>195</v>
+      </c>
+      <c r="I22" t="s">
+        <v>196</v>
+      </c>
+      <c r="J22" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>854</v>
+      </c>
+      <c r="B23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" t="s">
+        <v>199</v>
+      </c>
+      <c r="D23" t="s">
+        <v>200</v>
+      </c>
+      <c r="E23" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" t="s">
+        <v>201</v>
+      </c>
+      <c r="G23" t="s">
+        <v>202</v>
+      </c>
+      <c r="H23" t="s">
+        <v>203</v>
+      </c>
+      <c r="I23" t="s">
+        <v>204</v>
+      </c>
+      <c r="J23" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>855</v>
+      </c>
+      <c r="B24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" t="s">
+        <v>207</v>
+      </c>
+      <c r="D24" t="s">
+        <v>208</v>
+      </c>
+      <c r="E24" t="s">
+        <v>209</v>
+      </c>
+      <c r="F24" t="s">
+        <v>210</v>
+      </c>
+      <c r="G24" t="s">
+        <v>211</v>
+      </c>
+      <c r="H24" t="s">
+        <v>212</v>
+      </c>
+      <c r="I24" t="s">
+        <v>213</v>
+      </c>
+      <c r="J24" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>856</v>
+      </c>
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" t="s">
+        <v>216</v>
+      </c>
+      <c r="D25" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" t="s">
+        <v>217</v>
+      </c>
+      <c r="G25" t="s">
+        <v>218</v>
+      </c>
+      <c r="H25" t="s">
+        <v>219</v>
+      </c>
+      <c r="I25" t="s">
+        <v>220</v>
+      </c>
+      <c r="J25" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>857</v>
+      </c>
+      <c r="B26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" t="s">
+        <v>223</v>
+      </c>
+      <c r="D26" t="s">
+        <v>224</v>
+      </c>
+      <c r="E26" t="s">
+        <v>225</v>
+      </c>
+      <c r="F26" t="s">
+        <v>226</v>
+      </c>
+      <c r="G26" t="s">
+        <v>227</v>
+      </c>
+      <c r="H26" t="s">
+        <v>228</v>
+      </c>
+      <c r="I26" t="s">
+        <v>229</v>
+      </c>
+      <c r="J26" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>858</v>
+      </c>
+      <c r="B27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" t="s">
+        <v>232</v>
+      </c>
+      <c r="D27" t="s">
+        <v>233</v>
+      </c>
+      <c r="E27" t="s">
+        <v>192</v>
+      </c>
+      <c r="F27" t="s">
+        <v>234</v>
+      </c>
+      <c r="G27" t="s">
+        <v>235</v>
+      </c>
+      <c r="H27" t="s">
+        <v>236</v>
+      </c>
+      <c r="I27" t="s">
+        <v>237</v>
+      </c>
+      <c r="J27" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>859</v>
+      </c>
+      <c r="B28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" t="s">
+        <v>240</v>
+      </c>
+      <c r="D28" t="s">
+        <v>241</v>
+      </c>
+      <c r="E28" t="s">
+        <v>242</v>
+      </c>
+      <c r="F28" t="s">
+        <v>243</v>
+      </c>
+      <c r="G28" t="s">
+        <v>244</v>
+      </c>
+      <c r="H28" t="s">
+        <v>245</v>
+      </c>
+      <c r="I28" t="s">
+        <v>246</v>
+      </c>
+      <c r="J28" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>860</v>
+      </c>
+      <c r="B29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" t="s">
+        <v>249</v>
+      </c>
+      <c r="D29" t="s">
+        <v>140</v>
+      </c>
+      <c r="E29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" t="s">
+        <v>250</v>
+      </c>
+      <c r="G29" t="s">
+        <v>251</v>
+      </c>
+      <c r="H29" t="s">
+        <v>252</v>
+      </c>
+      <c r="I29" t="s">
+        <v>253</v>
+      </c>
+      <c r="J29" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>861</v>
+      </c>
+      <c r="B30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" t="s">
+        <v>256</v>
+      </c>
+      <c r="D30" t="s">
+        <v>257</v>
+      </c>
+      <c r="E30" t="s">
+        <v>258</v>
+      </c>
+      <c r="F30" t="s">
+        <v>259</v>
+      </c>
+      <c r="G30" t="s">
+        <v>260</v>
+      </c>
+      <c r="H30" t="s">
+        <v>261</v>
+      </c>
+      <c r="I30" t="s">
+        <v>262</v>
+      </c>
+      <c r="J30" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>862</v>
+      </c>
+      <c r="B31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" t="s">
+        <v>265</v>
+      </c>
+      <c r="D31" t="s">
+        <v>174</v>
+      </c>
+      <c r="E31" t="s">
+        <v>175</v>
+      </c>
+      <c r="F31" t="s">
+        <v>266</v>
+      </c>
+      <c r="G31" t="s">
+        <v>267</v>
+      </c>
+      <c r="H31" t="s">
+        <v>268</v>
+      </c>
+      <c r="I31" t="s">
+        <v>269</v>
+      </c>
+      <c r="J31" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>863</v>
+      </c>
+      <c r="B32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" t="s">
+        <v>272</v>
+      </c>
+      <c r="D32" t="s">
+        <v>273</v>
+      </c>
+      <c r="E32" t="s">
+        <v>192</v>
+      </c>
+      <c r="F32" t="s">
+        <v>274</v>
+      </c>
+      <c r="G32" t="s">
+        <v>275</v>
+      </c>
+      <c r="H32" t="s">
+        <v>276</v>
+      </c>
+      <c r="I32" t="s">
+        <v>277</v>
+      </c>
+      <c r="J32" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>864</v>
+      </c>
+      <c r="B33" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" t="s">
+        <v>280</v>
+      </c>
+      <c r="D33" t="s">
+        <v>148</v>
+      </c>
+      <c r="E33" t="s">
+        <v>149</v>
+      </c>
+      <c r="F33" t="s">
+        <v>281</v>
+      </c>
+      <c r="G33" t="s">
+        <v>282</v>
+      </c>
+      <c r="H33" t="s">
+        <v>283</v>
+      </c>
+      <c r="I33" t="s">
+        <v>284</v>
+      </c>
+      <c r="J33" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>865</v>
+      </c>
+      <c r="B34" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" t="s">
+        <v>287</v>
+      </c>
+      <c r="D34" t="s">
+        <v>288</v>
+      </c>
+      <c r="E34" t="s">
+        <v>60</v>
+      </c>
+      <c r="F34" t="s">
+        <v>289</v>
+      </c>
+      <c r="G34" t="s">
+        <v>290</v>
+      </c>
+      <c r="H34" t="s">
+        <v>291</v>
+      </c>
+      <c r="I34" t="s">
+        <v>292</v>
+      </c>
+      <c r="J34" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>866</v>
+      </c>
+      <c r="B35" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" t="s">
+        <v>295</v>
+      </c>
+      <c r="D35" t="s">
+        <v>296</v>
+      </c>
+      <c r="E35" t="s">
+        <v>69</v>
+      </c>
+      <c r="F35" t="s">
+        <v>297</v>
+      </c>
+      <c r="G35" t="s">
+        <v>298</v>
+      </c>
+      <c r="H35" t="s">
+        <v>299</v>
+      </c>
+      <c r="I35" t="s">
+        <v>300</v>
+      </c>
+      <c r="J35" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>867</v>
+      </c>
+      <c r="B36" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" t="s">
+        <v>303</v>
+      </c>
+      <c r="D36" t="s">
+        <v>304</v>
+      </c>
+      <c r="E36" t="s">
+        <v>149</v>
+      </c>
+      <c r="F36" t="s">
+        <v>305</v>
+      </c>
+      <c r="G36" t="s">
+        <v>306</v>
+      </c>
+      <c r="H36" t="s">
+        <v>307</v>
+      </c>
+      <c r="I36" t="s">
+        <v>308</v>
+      </c>
+      <c r="J36" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>868</v>
+      </c>
+      <c r="B37" t="s">
+        <v>22</v>
+      </c>
+      <c r="C37" t="s">
+        <v>311</v>
+      </c>
+      <c r="D37" t="s">
+        <v>312</v>
+      </c>
+      <c r="E37" t="s">
+        <v>96</v>
+      </c>
+      <c r="F37" t="s">
+        <v>313</v>
+      </c>
+      <c r="G37" t="s">
+        <v>314</v>
+      </c>
+      <c r="H37" t="s">
+        <v>315</v>
+      </c>
+      <c r="I37" t="s">
+        <v>316</v>
+      </c>
+      <c r="J37" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>869</v>
+      </c>
+      <c r="B38" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38" t="s">
+        <v>319</v>
+      </c>
+      <c r="D38" t="s">
+        <v>320</v>
+      </c>
+      <c r="E38" t="s">
+        <v>321</v>
+      </c>
+      <c r="F38" t="s">
+        <v>322</v>
+      </c>
+      <c r="G38" t="s">
+        <v>323</v>
+      </c>
+      <c r="H38" t="s">
+        <v>324</v>
+      </c>
+      <c r="I38" t="s">
+        <v>325</v>
+      </c>
+      <c r="J38" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>870</v>
+      </c>
+      <c r="B39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" t="s">
+        <v>328</v>
+      </c>
+      <c r="D39" t="s">
+        <v>122</v>
+      </c>
+      <c r="E39" t="s">
+        <v>329</v>
+      </c>
+      <c r="F39" t="s">
+        <v>330</v>
+      </c>
+      <c r="G39" t="s">
+        <v>331</v>
+      </c>
+      <c r="H39" t="s">
+        <v>332</v>
+      </c>
+      <c r="I39" t="s">
+        <v>333</v>
+      </c>
+      <c r="J39" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>871</v>
+      </c>
+      <c r="B40" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" t="s">
+        <v>336</v>
+      </c>
+      <c r="D40" t="s">
+        <v>337</v>
+      </c>
+      <c r="E40" t="s">
+        <v>338</v>
+      </c>
+      <c r="F40" t="s">
+        <v>339</v>
+      </c>
+      <c r="G40" t="s">
+        <v>340</v>
+      </c>
+      <c r="H40" t="s">
+        <v>341</v>
+      </c>
+      <c r="I40" t="s">
+        <v>342</v>
+      </c>
+      <c r="J40" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>872</v>
+      </c>
+      <c r="B41" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" t="s">
+        <v>345</v>
+      </c>
+      <c r="D41" t="s">
+        <v>346</v>
+      </c>
+      <c r="E41" t="s">
+        <v>347</v>
+      </c>
+      <c r="F41" t="s">
+        <v>348</v>
+      </c>
+      <c r="G41" t="s">
+        <v>349</v>
+      </c>
+      <c r="H41" t="s">
+        <v>350</v>
+      </c>
+      <c r="I41" t="s">
+        <v>351</v>
+      </c>
+      <c r="J41" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>873</v>
+      </c>
+      <c r="B42" t="s">
+        <v>22</v>
+      </c>
+      <c r="C42" t="s">
+        <v>354</v>
+      </c>
+      <c r="D42" t="s">
+        <v>355</v>
+      </c>
+      <c r="E42" t="s">
+        <v>114</v>
+      </c>
+      <c r="F42" t="s">
+        <v>356</v>
+      </c>
+      <c r="G42" t="s">
+        <v>357</v>
+      </c>
+      <c r="H42" t="s">
+        <v>358</v>
+      </c>
+      <c r="I42" t="s">
+        <v>359</v>
+      </c>
+      <c r="J42" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>874</v>
+      </c>
+      <c r="B43" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43" t="s">
+        <v>362</v>
+      </c>
+      <c r="D43" t="s">
+        <v>363</v>
+      </c>
+      <c r="E43" t="s">
+        <v>192</v>
+      </c>
+      <c r="F43" t="s">
+        <v>364</v>
+      </c>
+      <c r="G43" t="s">
+        <v>365</v>
+      </c>
+      <c r="H43" t="s">
+        <v>366</v>
+      </c>
+      <c r="I43" t="s">
+        <v>367</v>
+      </c>
+      <c r="J43" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>875</v>
+      </c>
+      <c r="B44" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" t="s">
+        <v>370</v>
+      </c>
+      <c r="D44" t="s">
+        <v>371</v>
+      </c>
+      <c r="E44" t="s">
+        <v>132</v>
+      </c>
+      <c r="F44" t="s">
+        <v>372</v>
+      </c>
+      <c r="G44" t="s">
+        <v>373</v>
+      </c>
+      <c r="H44" t="s">
+        <v>374</v>
+      </c>
+      <c r="I44" t="s">
+        <v>375</v>
+      </c>
+      <c r="J44" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>876</v>
+      </c>
+      <c r="B45" t="s">
+        <v>22</v>
+      </c>
+      <c r="C45" t="s">
+        <v>378</v>
+      </c>
+      <c r="D45" t="s">
+        <v>379</v>
+      </c>
+      <c r="E45" t="s">
+        <v>105</v>
+      </c>
+      <c r="F45" t="s">
+        <v>380</v>
+      </c>
+      <c r="G45" t="s">
+        <v>381</v>
+      </c>
+      <c r="H45" t="s">
+        <v>382</v>
+      </c>
+      <c r="I45" t="s">
+        <v>383</v>
+      </c>
+      <c r="J45" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>877</v>
+      </c>
+      <c r="B46" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46" t="s">
+        <v>386</v>
+      </c>
+      <c r="D46" t="s">
+        <v>387</v>
+      </c>
+      <c r="E46" t="s">
+        <v>388</v>
+      </c>
+      <c r="F46" t="s">
+        <v>389</v>
+      </c>
+      <c r="G46" t="s">
+        <v>390</v>
+      </c>
+      <c r="H46" t="s">
+        <v>391</v>
+      </c>
+      <c r="I46" t="s">
+        <v>392</v>
+      </c>
+      <c r="J46" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>878</v>
+      </c>
+      <c r="B47" t="s">
+        <v>22</v>
+      </c>
+      <c r="C47" t="s">
+        <v>395</v>
+      </c>
+      <c r="D47" t="s">
+        <v>396</v>
+      </c>
+      <c r="E47" t="s">
+        <v>397</v>
+      </c>
+      <c r="F47" t="s">
+        <v>398</v>
+      </c>
+      <c r="G47" t="s">
+        <v>399</v>
+      </c>
+      <c r="H47" t="s">
+        <v>400</v>
+      </c>
+      <c r="I47" t="s">
+        <v>401</v>
+      </c>
+      <c r="J47" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>879</v>
+      </c>
+      <c r="B48" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" t="s">
+        <v>404</v>
+      </c>
+      <c r="D48" t="s">
+        <v>33</v>
+      </c>
+      <c r="E48" t="s">
+        <v>15</v>
+      </c>
+      <c r="F48" t="s">
+        <v>405</v>
+      </c>
+      <c r="G48" t="s">
+        <v>406</v>
+      </c>
+      <c r="H48" t="s">
+        <v>407</v>
+      </c>
+      <c r="I48" t="s">
+        <v>408</v>
+      </c>
+      <c r="J48" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>880</v>
+      </c>
+      <c r="B49" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49" t="s">
+        <v>411</v>
+      </c>
+      <c r="D49" t="s">
+        <v>412</v>
+      </c>
+      <c r="E49" t="s">
+        <v>149</v>
+      </c>
+      <c r="F49" t="s">
+        <v>413</v>
+      </c>
+      <c r="G49" t="s">
+        <v>414</v>
+      </c>
+      <c r="H49" t="s">
+        <v>415</v>
+      </c>
+      <c r="I49" t="s">
+        <v>416</v>
+      </c>
+      <c r="J49" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>881</v>
+      </c>
+      <c r="B50" t="s">
+        <v>22</v>
+      </c>
+      <c r="C50" t="s">
+        <v>419</v>
+      </c>
+      <c r="D50" t="s">
+        <v>420</v>
+      </c>
+      <c r="E50" t="s">
+        <v>421</v>
+      </c>
+      <c r="F50" t="s">
+        <v>422</v>
+      </c>
+      <c r="G50" t="s">
+        <v>423</v>
+      </c>
+      <c r="H50" t="s">
+        <v>424</v>
+      </c>
+      <c r="I50" t="s">
+        <v>425</v>
+      </c>
+      <c r="J50" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>882</v>
+      </c>
+      <c r="B51" t="s">
+        <v>22</v>
+      </c>
+      <c r="C51" t="s">
+        <v>428</v>
+      </c>
+      <c r="D51" t="s">
+        <v>429</v>
+      </c>
+      <c r="E51" t="s">
+        <v>123</v>
+      </c>
+      <c r="F51" t="s">
+        <v>430</v>
+      </c>
+      <c r="G51" t="s">
+        <v>431</v>
+      </c>
+      <c r="H51" t="s">
+        <v>432</v>
+      </c>
+      <c r="I51" t="s">
+        <v>433</v>
+      </c>
+      <c r="J51" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>883</v>
+      </c>
+      <c r="B52" t="s">
+        <v>12</v>
+      </c>
+      <c r="C52" t="s">
+        <v>436</v>
+      </c>
+      <c r="D52" t="s">
+        <v>208</v>
+      </c>
+      <c r="E52" t="s">
+        <v>209</v>
+      </c>
+      <c r="F52" t="s">
+        <v>437</v>
+      </c>
+      <c r="G52" t="s">
+        <v>438</v>
+      </c>
+      <c r="H52" t="s">
+        <v>439</v>
+      </c>
+      <c r="I52" t="s">
+        <v>440</v>
+      </c>
+      <c r="J52" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>884</v>
+      </c>
+      <c r="B53" t="s">
+        <v>22</v>
+      </c>
+      <c r="C53" t="s">
+        <v>443</v>
+      </c>
+      <c r="D53" t="s">
+        <v>444</v>
+      </c>
+      <c r="E53" t="s">
+        <v>445</v>
+      </c>
+      <c r="F53" t="s">
+        <v>446</v>
+      </c>
+      <c r="G53" t="s">
+        <v>447</v>
+      </c>
+      <c r="H53" t="s">
+        <v>448</v>
+      </c>
+      <c r="I53" t="s">
+        <v>449</v>
+      </c>
+      <c r="J53" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>885</v>
+      </c>
+      <c r="B54" t="s">
+        <v>22</v>
+      </c>
+      <c r="C54" t="s">
+        <v>452</v>
+      </c>
+      <c r="D54" t="s">
+        <v>453</v>
+      </c>
+      <c r="E54" t="s">
+        <v>105</v>
+      </c>
+      <c r="F54" t="s">
+        <v>454</v>
+      </c>
+      <c r="G54" t="s">
+        <v>455</v>
+      </c>
+      <c r="H54" t="s">
+        <v>456</v>
+      </c>
+      <c r="I54" t="s">
+        <v>457</v>
+      </c>
+      <c r="J54" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>886</v>
+      </c>
+      <c r="B55" t="s">
+        <v>22</v>
+      </c>
+      <c r="C55" t="s">
+        <v>460</v>
+      </c>
+      <c r="D55" t="s">
+        <v>461</v>
+      </c>
+      <c r="E55" t="s">
+        <v>329</v>
+      </c>
+      <c r="F55" t="s">
+        <v>462</v>
+      </c>
+      <c r="G55" t="s">
+        <v>463</v>
+      </c>
+      <c r="H55" t="s">
+        <v>464</v>
+      </c>
+      <c r="I55" t="s">
+        <v>465</v>
+      </c>
+      <c r="J55" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>887</v>
+      </c>
+      <c r="B56" t="s">
+        <v>22</v>
+      </c>
+      <c r="C56" t="s">
+        <v>467</v>
+      </c>
+      <c r="D56" t="s">
+        <v>468</v>
+      </c>
+      <c r="E56" t="s">
+        <v>469</v>
+      </c>
+      <c r="F56" t="s">
+        <v>470</v>
+      </c>
+      <c r="G56" t="s">
+        <v>471</v>
+      </c>
+      <c r="H56" t="s">
+        <v>472</v>
+      </c>
+      <c r="I56" t="s">
+        <v>473</v>
+      </c>
+      <c r="J56" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>888</v>
+      </c>
+      <c r="B57" t="s">
+        <v>12</v>
+      </c>
+      <c r="C57" t="s">
+        <v>476</v>
+      </c>
+      <c r="D57" t="s">
+        <v>477</v>
+      </c>
+      <c r="E57" t="s">
+        <v>114</v>
+      </c>
+      <c r="F57" t="s">
+        <v>478</v>
+      </c>
+      <c r="G57" t="s">
+        <v>479</v>
+      </c>
+      <c r="H57" t="s">
+        <v>480</v>
+      </c>
+      <c r="I57" t="s">
+        <v>481</v>
+      </c>
+      <c r="J57" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>889</v>
+      </c>
+      <c r="B58" t="s">
+        <v>12</v>
+      </c>
+      <c r="C58" t="s">
+        <v>484</v>
+      </c>
+      <c r="D58" t="s">
+        <v>208</v>
+      </c>
+      <c r="E58" t="s">
+        <v>209</v>
+      </c>
+      <c r="F58" t="s">
+        <v>485</v>
+      </c>
+      <c r="G58" t="s">
+        <v>486</v>
+      </c>
+      <c r="H58" t="s">
+        <v>487</v>
+      </c>
+      <c r="I58" t="s">
+        <v>488</v>
+      </c>
+      <c r="J58" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>890</v>
+      </c>
+      <c r="B59" t="s">
+        <v>12</v>
+      </c>
+      <c r="C59" t="s">
+        <v>491</v>
+      </c>
+      <c r="D59" t="s">
+        <v>492</v>
+      </c>
+      <c r="E59" t="s">
+        <v>60</v>
+      </c>
+      <c r="F59" t="s">
+        <v>493</v>
+      </c>
+      <c r="G59" t="s">
+        <v>494</v>
+      </c>
+      <c r="H59" t="s">
+        <v>495</v>
+      </c>
+      <c r="I59" t="s">
+        <v>496</v>
+      </c>
+      <c r="J59" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>891</v>
+      </c>
+      <c r="B60" t="s">
+        <v>12</v>
+      </c>
+      <c r="C60" t="s">
+        <v>499</v>
+      </c>
+      <c r="D60" t="s">
+        <v>500</v>
+      </c>
+      <c r="E60" t="s">
+        <v>501</v>
+      </c>
+      <c r="F60" t="s">
+        <v>502</v>
+      </c>
+      <c r="G60" t="s">
+        <v>503</v>
+      </c>
+      <c r="H60" t="s">
+        <v>504</v>
+      </c>
+      <c r="I60" t="s">
+        <v>505</v>
+      </c>
+      <c r="J60" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>892</v>
+      </c>
+      <c r="B61" t="s">
+        <v>22</v>
+      </c>
+      <c r="C61" t="s">
+        <v>508</v>
+      </c>
+      <c r="D61" t="s">
+        <v>509</v>
+      </c>
+      <c r="E61" t="s">
+        <v>192</v>
+      </c>
+      <c r="F61" t="s">
+        <v>510</v>
+      </c>
+      <c r="G61" t="s">
+        <v>511</v>
+      </c>
+      <c r="H61" t="s">
+        <v>512</v>
+      </c>
+      <c r="I61" t="s">
+        <v>513</v>
+      </c>
+      <c r="J61" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>893</v>
+      </c>
+      <c r="B62" t="s">
+        <v>22</v>
+      </c>
+      <c r="C62" t="s">
+        <v>516</v>
+      </c>
+      <c r="D62" t="s">
+        <v>208</v>
+      </c>
+      <c r="E62" t="s">
+        <v>209</v>
+      </c>
+      <c r="F62" t="s">
+        <v>517</v>
+      </c>
+      <c r="G62" t="s">
+        <v>518</v>
+      </c>
+      <c r="H62" t="s">
+        <v>519</v>
+      </c>
+      <c r="I62" t="s">
+        <v>520</v>
+      </c>
+      <c r="J62" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>894</v>
+      </c>
+      <c r="B63" t="s">
+        <v>12</v>
+      </c>
+      <c r="C63" t="s">
+        <v>523</v>
+      </c>
+      <c r="D63" t="s">
+        <v>183</v>
+      </c>
+      <c r="E63" t="s">
+        <v>123</v>
+      </c>
+      <c r="F63" t="s">
+        <v>524</v>
+      </c>
+      <c r="G63" t="s">
+        <v>525</v>
+      </c>
+      <c r="H63" t="s">
+        <v>526</v>
+      </c>
+      <c r="I63" t="s">
+        <v>527</v>
+      </c>
+      <c r="J63" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>895</v>
+      </c>
+      <c r="B64" t="s">
+        <v>12</v>
+      </c>
+      <c r="C64" t="s">
+        <v>530</v>
+      </c>
+      <c r="D64" t="s">
+        <v>140</v>
+      </c>
+      <c r="E64" t="s">
+        <v>15</v>
+      </c>
+      <c r="F64" t="s">
+        <v>531</v>
+      </c>
+      <c r="G64" t="s">
+        <v>532</v>
+      </c>
+      <c r="H64" t="s">
+        <v>533</v>
+      </c>
+      <c r="I64" t="s">
+        <v>534</v>
+      </c>
+      <c r="J64" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>896</v>
+      </c>
+      <c r="B65" t="s">
+        <v>12</v>
+      </c>
+      <c r="C65" t="s">
+        <v>537</v>
+      </c>
+      <c r="D65" t="s">
+        <v>538</v>
+      </c>
+      <c r="E65" t="s">
+        <v>445</v>
+      </c>
+      <c r="F65" t="s">
+        <v>539</v>
+      </c>
+      <c r="G65" t="s">
+        <v>540</v>
+      </c>
+      <c r="H65" t="s">
+        <v>541</v>
+      </c>
+      <c r="I65" t="s">
+        <v>542</v>
+      </c>
+      <c r="J65" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>897</v>
+      </c>
+      <c r="B66" t="s">
+        <v>22</v>
+      </c>
+      <c r="C66" t="s">
+        <v>545</v>
+      </c>
+      <c r="D66" t="s">
+        <v>208</v>
+      </c>
+      <c r="E66" t="s">
+        <v>209</v>
+      </c>
+      <c r="F66" t="s">
+        <v>546</v>
+      </c>
+      <c r="G66" t="s">
+        <v>547</v>
+      </c>
+      <c r="H66" t="s">
+        <v>548</v>
+      </c>
+      <c r="I66" t="s">
+        <v>549</v>
+      </c>
+      <c r="J66" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>898</v>
+      </c>
+      <c r="B67" t="s">
+        <v>22</v>
+      </c>
+      <c r="C67" t="s">
+        <v>552</v>
+      </c>
+      <c r="D67" t="s">
+        <v>553</v>
+      </c>
+      <c r="E67" t="s">
+        <v>149</v>
+      </c>
+      <c r="F67" t="s">
+        <v>554</v>
+      </c>
+      <c r="G67" t="s">
+        <v>555</v>
+      </c>
+      <c r="H67" t="s">
+        <v>556</v>
+      </c>
+      <c r="I67" t="s">
+        <v>557</v>
+      </c>
+      <c r="J67" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>899</v>
+      </c>
+      <c r="B68" t="s">
+        <v>12</v>
+      </c>
+      <c r="C68" t="s">
+        <v>560</v>
+      </c>
+      <c r="D68" t="s">
+        <v>561</v>
+      </c>
+      <c r="E68" t="s">
+        <v>69</v>
+      </c>
+      <c r="F68" t="s">
+        <v>562</v>
+      </c>
+      <c r="G68" t="s">
+        <v>563</v>
+      </c>
+      <c r="H68" t="s">
+        <v>564</v>
+      </c>
+      <c r="I68" t="s">
+        <v>565</v>
+      </c>
+      <c r="J68" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>900</v>
+      </c>
+      <c r="B69" t="s">
+        <v>22</v>
+      </c>
+      <c r="C69" t="s">
+        <v>568</v>
+      </c>
+      <c r="D69" t="s">
+        <v>569</v>
+      </c>
+      <c r="E69" t="s">
+        <v>42</v>
+      </c>
+      <c r="F69" t="s">
+        <v>570</v>
+      </c>
+      <c r="G69" t="s">
+        <v>571</v>
+      </c>
+      <c r="H69" t="s">
+        <v>572</v>
+      </c>
+      <c r="I69" t="s">
+        <v>573</v>
+      </c>
+      <c r="J69" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>901</v>
+      </c>
+      <c r="B70" t="s">
+        <v>12</v>
+      </c>
+      <c r="C70" t="s">
+        <v>576</v>
+      </c>
+      <c r="D70" t="s">
+        <v>577</v>
+      </c>
+      <c r="E70" t="s">
+        <v>578</v>
+      </c>
+      <c r="F70" t="s">
+        <v>579</v>
+      </c>
+      <c r="G70" t="s">
+        <v>580</v>
+      </c>
+      <c r="H70" t="s">
+        <v>581</v>
+      </c>
+      <c r="I70" t="s">
+        <v>582</v>
+      </c>
+      <c r="J70" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>902</v>
+      </c>
+      <c r="B71" t="s">
+        <v>22</v>
+      </c>
+      <c r="C71" t="s">
+        <v>585</v>
+      </c>
+      <c r="D71" t="s">
+        <v>586</v>
+      </c>
+      <c r="E71" t="s">
+        <v>587</v>
+      </c>
+      <c r="F71" t="s">
+        <v>588</v>
+      </c>
+      <c r="G71" t="s">
+        <v>589</v>
+      </c>
+      <c r="H71" t="s">
+        <v>590</v>
+      </c>
+      <c r="I71" t="s">
+        <v>591</v>
+      </c>
+      <c r="J71" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>903</v>
+      </c>
+      <c r="B72" t="s">
+        <v>12</v>
+      </c>
+      <c r="C72" t="s">
+        <v>594</v>
+      </c>
+      <c r="D72" t="s">
+        <v>595</v>
+      </c>
+      <c r="E72" t="s">
+        <v>469</v>
+      </c>
+      <c r="F72" t="s">
+        <v>596</v>
+      </c>
+      <c r="G72" t="s">
+        <v>597</v>
+      </c>
+      <c r="H72" t="s">
+        <v>598</v>
+      </c>
+      <c r="I72" t="s">
+        <v>599</v>
+      </c>
+      <c r="J72" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>904</v>
+      </c>
+      <c r="B73" t="s">
+        <v>22</v>
+      </c>
+      <c r="C73" t="s">
+        <v>602</v>
+      </c>
+      <c r="D73" t="s">
+        <v>603</v>
+      </c>
+      <c r="E73" t="s">
+        <v>15</v>
+      </c>
+      <c r="F73" t="s">
+        <v>604</v>
+      </c>
+      <c r="G73" t="s">
+        <v>605</v>
+      </c>
+      <c r="H73" t="s">
+        <v>606</v>
+      </c>
+      <c r="I73" t="s">
+        <v>607</v>
+      </c>
+      <c r="J73" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>905</v>
+      </c>
+      <c r="B74" t="s">
+        <v>22</v>
+      </c>
+      <c r="C74" t="s">
+        <v>610</v>
+      </c>
+      <c r="D74" t="s">
+        <v>611</v>
+      </c>
+      <c r="E74" t="s">
+        <v>242</v>
+      </c>
+      <c r="F74" t="s">
+        <v>612</v>
+      </c>
+      <c r="G74" t="s">
+        <v>613</v>
+      </c>
+      <c r="H74" t="s">
+        <v>614</v>
+      </c>
+      <c r="I74" t="s">
+        <v>615</v>
+      </c>
+      <c r="J74" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>906</v>
+      </c>
+      <c r="B75" t="s">
+        <v>22</v>
+      </c>
+      <c r="C75" t="s">
+        <v>618</v>
+      </c>
+      <c r="D75" t="s">
+        <v>619</v>
+      </c>
+      <c r="E75" t="s">
+        <v>132</v>
+      </c>
+      <c r="F75" t="s">
+        <v>620</v>
+      </c>
+      <c r="G75" t="s">
+        <v>621</v>
+      </c>
+      <c r="H75" t="s">
+        <v>622</v>
+      </c>
+      <c r="I75" t="s">
+        <v>623</v>
+      </c>
+      <c r="J75" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>907</v>
+      </c>
+      <c r="B76" t="s">
+        <v>22</v>
+      </c>
+      <c r="C76" t="s">
+        <v>626</v>
+      </c>
+      <c r="D76" t="s">
+        <v>627</v>
+      </c>
+      <c r="E76" t="s">
+        <v>25</v>
+      </c>
+      <c r="F76" t="s">
+        <v>628</v>
+      </c>
+      <c r="G76" t="s">
+        <v>629</v>
+      </c>
+      <c r="H76" t="s">
+        <v>630</v>
+      </c>
+      <c r="I76" t="s">
+        <v>631</v>
+      </c>
+      <c r="J76" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>908</v>
+      </c>
+      <c r="B77" t="s">
+        <v>22</v>
+      </c>
+      <c r="C77" t="s">
+        <v>634</v>
+      </c>
+      <c r="D77" t="s">
+        <v>635</v>
+      </c>
+      <c r="E77" t="s">
+        <v>105</v>
+      </c>
+      <c r="F77" t="s">
+        <v>636</v>
+      </c>
+      <c r="G77" t="s">
+        <v>637</v>
+      </c>
+      <c r="H77" t="s">
+        <v>638</v>
+      </c>
+      <c r="I77" t="s">
+        <v>639</v>
+      </c>
+      <c r="J77" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>909</v>
+      </c>
+      <c r="B78" t="s">
+        <v>22</v>
+      </c>
+      <c r="C78" t="s">
+        <v>642</v>
+      </c>
+      <c r="D78" t="s">
+        <v>643</v>
+      </c>
+      <c r="E78" t="s">
+        <v>60</v>
+      </c>
+      <c r="F78" t="s">
+        <v>644</v>
+      </c>
+      <c r="G78" t="s">
+        <v>645</v>
+      </c>
+      <c r="H78" t="s">
+        <v>646</v>
+      </c>
+      <c r="I78" t="s">
+        <v>647</v>
+      </c>
+      <c r="J78" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>910</v>
+      </c>
+      <c r="B79" t="s">
+        <v>12</v>
+      </c>
+      <c r="C79" t="s">
+        <v>650</v>
+      </c>
+      <c r="D79" t="s">
+        <v>643</v>
+      </c>
+      <c r="E79" t="s">
+        <v>60</v>
+      </c>
+      <c r="F79" t="s">
+        <v>651</v>
+      </c>
+      <c r="G79" t="s">
+        <v>652</v>
+      </c>
+      <c r="H79" t="s">
+        <v>653</v>
+      </c>
+      <c r="I79" t="s">
+        <v>654</v>
+      </c>
+      <c r="J79" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>911</v>
+      </c>
+      <c r="B80" t="s">
+        <v>22</v>
+      </c>
+      <c r="C80" t="s">
+        <v>657</v>
+      </c>
+      <c r="D80" t="s">
+        <v>658</v>
+      </c>
+      <c r="E80" t="s">
+        <v>15</v>
+      </c>
+      <c r="F80" t="s">
+        <v>659</v>
+      </c>
+      <c r="G80" t="s">
+        <v>660</v>
+      </c>
+      <c r="H80" t="s">
+        <v>661</v>
+      </c>
+      <c r="I80" t="s">
+        <v>662</v>
+      </c>
+      <c r="J80" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>912</v>
+      </c>
+      <c r="B81" t="s">
+        <v>22</v>
+      </c>
+      <c r="C81" t="s">
+        <v>665</v>
+      </c>
+      <c r="D81" t="s">
+        <v>666</v>
+      </c>
+      <c r="E81" t="s">
+        <v>667</v>
+      </c>
+      <c r="F81" t="s">
+        <v>668</v>
+      </c>
+      <c r="G81" t="s">
+        <v>669</v>
+      </c>
+      <c r="H81" t="s">
+        <v>670</v>
+      </c>
+      <c r="I81" t="s">
+        <v>671</v>
+      </c>
+      <c r="J81" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>913</v>
+      </c>
+      <c r="B82" t="s">
+        <v>12</v>
+      </c>
+      <c r="C82" t="s">
+        <v>674</v>
+      </c>
+      <c r="D82" t="s">
+        <v>200</v>
+      </c>
+      <c r="E82" t="s">
+        <v>25</v>
+      </c>
+      <c r="F82" t="s">
+        <v>675</v>
+      </c>
+      <c r="G82" t="s">
+        <v>676</v>
+      </c>
+      <c r="H82" t="s">
+        <v>677</v>
+      </c>
+      <c r="I82" t="s">
+        <v>678</v>
+      </c>
+      <c r="J82" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>914</v>
+      </c>
+      <c r="B83" t="s">
+        <v>22</v>
+      </c>
+      <c r="C83" t="s">
+        <v>681</v>
+      </c>
+      <c r="D83" t="s">
+        <v>682</v>
+      </c>
+      <c r="E83" t="s">
+        <v>587</v>
+      </c>
+      <c r="F83" t="s">
+        <v>683</v>
+      </c>
+      <c r="G83" t="s">
+        <v>684</v>
+      </c>
+      <c r="H83" t="s">
+        <v>685</v>
+      </c>
+      <c r="I83" t="s">
+        <v>686</v>
+      </c>
+      <c r="J83" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>915</v>
+      </c>
+      <c r="B84" t="s">
+        <v>22</v>
+      </c>
+      <c r="C84" t="s">
+        <v>689</v>
+      </c>
+      <c r="D84" t="s">
+        <v>690</v>
+      </c>
+      <c r="E84" t="s">
+        <v>15</v>
+      </c>
+      <c r="F84" t="s">
+        <v>691</v>
+      </c>
+      <c r="G84" t="s">
+        <v>692</v>
+      </c>
+      <c r="H84" t="s">
+        <v>693</v>
+      </c>
+      <c r="I84" t="s">
+        <v>694</v>
+      </c>
+      <c r="J84" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>916</v>
+      </c>
+      <c r="B85" t="s">
+        <v>12</v>
+      </c>
+      <c r="C85" t="s">
+        <v>697</v>
+      </c>
+      <c r="D85" t="s">
+        <v>698</v>
+      </c>
+      <c r="E85" t="s">
+        <v>699</v>
+      </c>
+      <c r="F85" t="s">
+        <v>700</v>
+      </c>
+      <c r="G85" t="s">
+        <v>701</v>
+      </c>
+      <c r="H85" t="s">
+        <v>702</v>
+      </c>
+      <c r="I85" t="s">
+        <v>703</v>
+      </c>
+      <c r="J85" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>917</v>
+      </c>
+      <c r="B86" t="s">
+        <v>22</v>
+      </c>
+      <c r="C86" t="s">
+        <v>706</v>
+      </c>
+      <c r="D86" t="s">
+        <v>707</v>
+      </c>
+      <c r="E86" t="s">
+        <v>132</v>
+      </c>
+      <c r="F86" t="s">
+        <v>708</v>
+      </c>
+      <c r="G86" t="s">
+        <v>709</v>
+      </c>
+      <c r="H86" t="s">
+        <v>710</v>
+      </c>
+      <c r="I86" t="s">
+        <v>711</v>
+      </c>
+      <c r="J86" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>918</v>
+      </c>
+      <c r="B87" t="s">
+        <v>12</v>
+      </c>
+      <c r="C87" t="s">
+        <v>714</v>
+      </c>
+      <c r="D87" t="s">
+        <v>371</v>
+      </c>
+      <c r="E87" t="s">
+        <v>132</v>
+      </c>
+      <c r="F87" t="s">
+        <v>715</v>
+      </c>
+      <c r="G87" t="s">
+        <v>716</v>
+      </c>
+      <c r="H87" t="s">
+        <v>717</v>
+      </c>
+      <c r="I87" t="s">
+        <v>718</v>
+      </c>
+      <c r="J87" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>919</v>
+      </c>
+      <c r="B88" t="s">
+        <v>22</v>
+      </c>
+      <c r="C88" t="s">
+        <v>721</v>
+      </c>
+      <c r="D88" t="s">
+        <v>722</v>
+      </c>
+      <c r="E88" t="s">
+        <v>501</v>
+      </c>
+      <c r="F88" t="s">
+        <v>723</v>
+      </c>
+      <c r="G88" t="s">
+        <v>724</v>
+      </c>
+      <c r="H88" t="s">
+        <v>725</v>
+      </c>
+      <c r="I88" t="s">
+        <v>726</v>
+      </c>
+      <c r="J88" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>920</v>
+      </c>
+      <c r="B89" t="s">
+        <v>12</v>
+      </c>
+      <c r="C89" t="s">
+        <v>729</v>
+      </c>
+      <c r="D89" t="s">
+        <v>730</v>
+      </c>
+      <c r="E89" t="s">
+        <v>132</v>
+      </c>
+      <c r="F89" t="s">
+        <v>731</v>
+      </c>
+      <c r="G89" t="s">
+        <v>732</v>
+      </c>
+      <c r="H89" t="s">
+        <v>733</v>
+      </c>
+      <c r="I89" t="s">
+        <v>734</v>
+      </c>
+      <c r="J89" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>921</v>
+      </c>
+      <c r="B90" t="s">
+        <v>12</v>
+      </c>
+      <c r="C90" t="s">
+        <v>737</v>
+      </c>
+      <c r="D90" t="s">
+        <v>738</v>
+      </c>
+      <c r="E90" t="s">
+        <v>192</v>
+      </c>
+      <c r="F90" t="s">
+        <v>739</v>
+      </c>
+      <c r="G90" t="s">
+        <v>740</v>
+      </c>
+      <c r="H90" t="s">
+        <v>741</v>
+      </c>
+      <c r="I90" t="s">
+        <v>742</v>
+      </c>
+      <c r="J90" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>922</v>
+      </c>
+      <c r="B91" t="s">
+        <v>22</v>
+      </c>
+      <c r="C91" t="s">
+        <v>745</v>
+      </c>
+      <c r="D91" t="s">
+        <v>746</v>
+      </c>
+      <c r="E91" t="s">
+        <v>69</v>
+      </c>
+      <c r="F91" t="s">
+        <v>747</v>
+      </c>
+      <c r="G91" t="s">
+        <v>748</v>
+      </c>
+      <c r="H91" t="s">
+        <v>749</v>
+      </c>
+      <c r="I91" t="s">
+        <v>750</v>
+      </c>
+      <c r="J91" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>923</v>
+      </c>
+      <c r="B92" t="s">
+        <v>12</v>
+      </c>
+      <c r="C92" t="s">
+        <v>753</v>
+      </c>
+      <c r="D92" t="s">
+        <v>754</v>
+      </c>
+      <c r="E92" t="s">
+        <v>388</v>
+      </c>
+      <c r="F92" t="s">
+        <v>755</v>
+      </c>
+      <c r="G92" t="s">
+        <v>756</v>
+      </c>
+      <c r="H92" t="s">
+        <v>757</v>
+      </c>
+      <c r="I92" t="s">
+        <v>758</v>
+      </c>
+      <c r="J92" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>924</v>
+      </c>
+      <c r="B93" t="s">
+        <v>12</v>
+      </c>
+      <c r="C93" t="s">
+        <v>761</v>
+      </c>
+      <c r="D93" t="s">
+        <v>762</v>
+      </c>
+      <c r="E93" t="s">
+        <v>60</v>
+      </c>
+      <c r="F93" t="s">
+        <v>763</v>
+      </c>
+      <c r="G93">
+        <v>-5208</v>
+      </c>
+      <c r="H93" t="s">
+        <v>764</v>
+      </c>
+      <c r="I93" t="s">
+        <v>765</v>
+      </c>
+      <c r="J93" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>925</v>
+      </c>
+      <c r="B94" t="s">
+        <v>22</v>
+      </c>
+      <c r="C94" t="s">
+        <v>768</v>
+      </c>
+      <c r="D94" t="s">
+        <v>769</v>
+      </c>
+      <c r="E94" t="s">
+        <v>208</v>
+      </c>
+      <c r="F94" t="s">
+        <v>770</v>
+      </c>
+      <c r="G94" t="s">
+        <v>771</v>
+      </c>
+      <c r="H94" t="s">
+        <v>772</v>
+      </c>
+      <c r="I94" t="s">
+        <v>773</v>
+      </c>
+      <c r="J94" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>926</v>
+      </c>
+      <c r="B95" t="s">
+        <v>12</v>
+      </c>
+      <c r="C95" t="s">
+        <v>776</v>
+      </c>
+      <c r="D95" t="s">
+        <v>777</v>
+      </c>
+      <c r="E95" t="s">
+        <v>778</v>
+      </c>
+      <c r="F95" t="s">
+        <v>779</v>
+      </c>
+      <c r="G95" t="s">
+        <v>780</v>
+      </c>
+      <c r="H95" t="s">
+        <v>781</v>
+      </c>
+      <c r="I95" t="s">
+        <v>782</v>
+      </c>
+      <c r="J95" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>927</v>
+      </c>
+      <c r="B96" t="s">
+        <v>22</v>
+      </c>
+      <c r="C96" t="s">
+        <v>785</v>
+      </c>
+      <c r="D96" t="s">
+        <v>698</v>
+      </c>
+      <c r="E96" t="s">
+        <v>699</v>
+      </c>
+      <c r="F96" t="s">
+        <v>786</v>
+      </c>
+      <c r="G96" t="s">
+        <v>787</v>
+      </c>
+      <c r="H96" t="s">
+        <v>788</v>
+      </c>
+      <c r="I96" t="s">
+        <v>789</v>
+      </c>
+      <c r="J96" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>928</v>
+      </c>
+      <c r="B97" t="s">
+        <v>22</v>
+      </c>
+      <c r="C97" t="s">
+        <v>792</v>
+      </c>
+      <c r="D97" t="s">
+        <v>793</v>
+      </c>
+      <c r="E97" t="s">
+        <v>192</v>
+      </c>
+      <c r="F97" t="s">
+        <v>794</v>
+      </c>
+      <c r="G97" t="s">
+        <v>795</v>
+      </c>
+      <c r="H97" t="s">
+        <v>796</v>
+      </c>
+      <c r="I97" t="s">
+        <v>797</v>
+      </c>
+      <c r="J97" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>929</v>
+      </c>
+      <c r="B98" t="s">
+        <v>22</v>
+      </c>
+      <c r="C98" t="s">
+        <v>800</v>
+      </c>
+      <c r="D98" t="s">
+        <v>429</v>
+      </c>
+      <c r="E98" t="s">
+        <v>123</v>
+      </c>
+      <c r="F98" t="s">
+        <v>801</v>
+      </c>
+      <c r="G98" t="s">
+        <v>802</v>
+      </c>
+      <c r="H98" t="s">
+        <v>803</v>
+      </c>
+      <c r="I98" t="s">
+        <v>804</v>
+      </c>
+      <c r="J98" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>930</v>
+      </c>
+      <c r="B99" t="s">
+        <v>22</v>
+      </c>
+      <c r="C99" t="s">
+        <v>807</v>
+      </c>
+      <c r="D99" t="s">
+        <v>808</v>
+      </c>
+      <c r="E99" t="s">
+        <v>149</v>
+      </c>
+      <c r="F99" t="s">
+        <v>809</v>
+      </c>
+      <c r="G99" t="s">
+        <v>810</v>
+      </c>
+      <c r="H99" t="s">
+        <v>811</v>
+      </c>
+      <c r="I99" t="s">
+        <v>812</v>
+      </c>
+      <c r="J99" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>931</v>
+      </c>
+      <c r="B100" t="s">
+        <v>12</v>
+      </c>
+      <c r="C100" t="s">
+        <v>815</v>
+      </c>
+      <c r="D100" t="s">
+        <v>816</v>
+      </c>
+      <c r="E100" t="s">
+        <v>258</v>
+      </c>
+      <c r="F100" t="s">
+        <v>817</v>
+      </c>
+      <c r="G100" t="s">
+        <v>818</v>
+      </c>
+      <c r="H100" t="s">
+        <v>819</v>
+      </c>
+      <c r="I100" t="s">
+        <v>820</v>
+      </c>
+      <c r="J100" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>932</v>
+      </c>
+      <c r="B101" t="s">
+        <v>22</v>
+      </c>
+      <c r="C101" t="s">
+        <v>823</v>
+      </c>
+      <c r="D101" t="s">
+        <v>824</v>
+      </c>
+      <c r="E101" t="s">
+        <v>51</v>
+      </c>
+      <c r="F101" t="s">
+        <v>825</v>
+      </c>
+      <c r="G101" t="s">
+        <v>826</v>
+      </c>
+      <c r="H101" t="s">
+        <v>827</v>
+      </c>
+      <c r="I101" t="s">
+        <v>828</v>
+      </c>
+      <c r="J101" t="s">
+        <v>834</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3398,7 +6956,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -3430,7 +6988,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -3462,7 +7020,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -3494,7 +7052,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -3526,7 +7084,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -3558,7 +7116,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -3590,7 +7148,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>65</v>
       </c>
@@ -3622,7 +7180,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>74</v>
       </c>
@@ -3654,7 +7212,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>83</v>
       </c>
@@ -3686,7 +7244,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>92</v>
       </c>
@@ -3718,7 +7276,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>101</v>
       </c>
@@ -3750,7 +7308,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>110</v>
       </c>
@@ -3782,7 +7340,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>119</v>
       </c>
@@ -3814,7 +7372,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>128</v>
       </c>
@@ -3846,7 +7404,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>137</v>
       </c>
@@ -3878,7 +7436,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>145</v>
       </c>
@@ -3910,7 +7468,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>154</v>
       </c>
@@ -3942,7 +7500,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>163</v>
       </c>
@@ -3974,7 +7532,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>171</v>
       </c>
@@ -4006,7 +7564,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>180</v>
       </c>
@@ -4038,7 +7596,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>188</v>
       </c>
@@ -4070,7 +7628,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>197</v>
       </c>
@@ -4102,7 +7660,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>205</v>
       </c>
@@ -4134,7 +7692,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>214</v>
       </c>
@@ -4166,7 +7724,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>221</v>
       </c>
@@ -4198,7 +7756,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>230</v>
       </c>
@@ -4230,7 +7788,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>238</v>
       </c>
@@ -4262,7 +7820,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>247</v>
       </c>
@@ -4294,7 +7852,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>254</v>
       </c>
@@ -4326,7 +7884,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>263</v>
       </c>
@@ -4358,7 +7916,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>270</v>
       </c>
@@ -4390,7 +7948,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>278</v>
       </c>
@@ -4422,7 +7980,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>285</v>
       </c>
@@ -4454,7 +8012,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>293</v>
       </c>
@@ -4486,7 +8044,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>301</v>
       </c>
@@ -4518,7 +8076,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>309</v>
       </c>
@@ -4550,7 +8108,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>317</v>
       </c>
@@ -4582,7 +8140,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>326</v>
       </c>
@@ -4614,7 +8172,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>334</v>
       </c>
@@ -4646,7 +8204,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>343</v>
       </c>
@@ -4678,7 +8236,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>352</v>
       </c>
@@ -4710,7 +8268,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>360</v>
       </c>
@@ -4742,7 +8300,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>368</v>
       </c>
@@ -4774,7 +8332,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>376</v>
       </c>
@@ -4806,7 +8364,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>384</v>
       </c>
@@ -4838,7 +8396,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>393</v>
       </c>
@@ -4870,7 +8428,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>402</v>
       </c>
@@ -4902,7 +8460,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>409</v>
       </c>
@@ -4934,7 +8492,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>417</v>
       </c>
@@ -4966,7 +8524,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>426</v>
       </c>
@@ -4998,7 +8556,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>434</v>
       </c>
@@ -5030,7 +8588,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>441</v>
       </c>
@@ -5062,7 +8620,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>450</v>
       </c>
@@ -5094,7 +8652,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>458</v>
       </c>
@@ -5126,7 +8684,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>101</v>
       </c>
@@ -5158,7 +8716,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>474</v>
       </c>
@@ -5190,7 +8748,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>482</v>
       </c>
@@ -5222,7 +8780,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>489</v>
       </c>
@@ -5254,7 +8812,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>497</v>
       </c>
@@ -5286,7 +8844,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>506</v>
       </c>
@@ -5318,7 +8876,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>514</v>
       </c>
@@ -5350,7 +8908,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>521</v>
       </c>
@@ -5382,7 +8940,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>528</v>
       </c>
@@ -5414,7 +8972,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>535</v>
       </c>
@@ -5446,7 +9004,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>543</v>
       </c>
@@ -5478,7 +9036,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>550</v>
       </c>
@@ -5510,7 +9068,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>558</v>
       </c>
@@ -5542,7 +9100,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>566</v>
       </c>
@@ -5574,7 +9132,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>574</v>
       </c>
@@ -5606,7 +9164,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>583</v>
       </c>
@@ -5638,7 +9196,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>592</v>
       </c>
@@ -5670,7 +9228,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>600</v>
       </c>
@@ -5702,7 +9260,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>608</v>
       </c>
@@ -5734,7 +9292,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>616</v>
       </c>
@@ -5766,7 +9324,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>624</v>
       </c>
@@ -5798,7 +9356,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>632</v>
       </c>
@@ -5830,7 +9388,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>640</v>
       </c>
@@ -5862,7 +9420,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>648</v>
       </c>
@@ -5894,7 +9452,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>655</v>
       </c>
@@ -5926,7 +9484,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>663</v>
       </c>
@@ -5958,7 +9516,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>672</v>
       </c>
@@ -5990,7 +9548,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>679</v>
       </c>
@@ -6022,7 +9580,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>687</v>
       </c>
@@ -6054,7 +9612,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>695</v>
       </c>
@@ -6086,7 +9644,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>704</v>
       </c>
@@ -6118,7 +9676,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>712</v>
       </c>
@@ -6150,7 +9708,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>719</v>
       </c>
@@ -6182,7 +9740,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>727</v>
       </c>
@@ -6214,7 +9772,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>735</v>
       </c>
@@ -6246,7 +9804,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>743</v>
       </c>
@@ -6278,7 +9836,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>751</v>
       </c>
@@ -6310,7 +9868,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>759</v>
       </c>
@@ -6342,7 +9900,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>766</v>
       </c>
@@ -6374,7 +9932,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>774</v>
       </c>
@@ -6406,7 +9964,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>783</v>
       </c>
@@ -6438,7 +9996,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>790</v>
       </c>
@@ -6470,7 +10028,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>798</v>
       </c>
@@ -6502,7 +10060,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>805</v>
       </c>
@@ -6534,7 +10092,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>813</v>
       </c>
@@ -6566,7 +10124,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>821</v>
       </c>

</xml_diff>